<commit_message>
Finished Query resuls excel sheet
</commit_message>
<xml_diff>
--- a/Project6_QueryResults.xlsx
+++ b/Project6_QueryResults.xlsx
@@ -173,13 +173,10 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="C10:L11"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -233,34 +230,34 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>0.775</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.755</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>0.775</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>0.78</v>
+        <v>0.815</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.775</v>
+        <v>0.785</v>
       </c>
       <c r="I2" s="1" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>0.795</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>0.79</v>
-      </c>
       <c r="K2" s="1" t="n">
-        <v>0.73</v>
+        <v>0.755</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="M2" s="1"/>
     </row>
@@ -269,34 +266,34 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.81</v>
+        <v>0.8365</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.825</v>
+        <v>0.739</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>0.745</v>
+        <v>0.7082</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.77</v>
+        <v>0.7854</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0.7555</v>
+        <v>0.7493</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.775</v>
+        <v>0.8192</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.795</v>
+        <v>0.732</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.765</v>
+        <v>0.7808</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.77</v>
+        <v>0.7734</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.785</v>
+        <v>0.7581</v>
       </c>
       <c r="M3" s="1"/>
     </row>
@@ -308,34 +305,34 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.7525</v>
+        <v>0.8</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0.775</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.8125</v>
+        <v>0.775</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.7525</v>
+        <v>0.7775</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.745</v>
+        <v>0.7675</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.7625</v>
+        <v>0.755</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.785</v>
+        <v>0.735</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.7775</v>
+        <v>0.735</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.775</v>
+        <v>0.7325</v>
       </c>
       <c r="M4" s="1"/>
     </row>
@@ -344,34 +341,34 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.7275</v>
+        <v>0.7742</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.825</v>
+        <v>0.7561</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0.7725</v>
+        <v>0.7442</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.71</v>
+        <v>0.8032</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.785</v>
+        <v>0.7623</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0.79</v>
+        <v>0.8058</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>0.7875</v>
+        <v>0.7801</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0.765</v>
+        <v>0.7006</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.7875</v>
+        <v>0.7471</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0.77</v>
+        <v>0.8218</v>
       </c>
       <c r="M5" s="1"/>
     </row>
@@ -383,34 +380,34 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0.7733</v>
+        <v>0.7567</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.7667</v>
+        <v>0.78</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>0.785</v>
+        <v>0.7833</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0.77</v>
+        <v>0.7517</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0.7683</v>
+        <v>0.745</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>0.7417</v>
+        <v>0.7633</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>0.7583</v>
+        <v>0.7767</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>0.7667</v>
+        <v>0.7883</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>0.7667</v>
+        <v>0.78</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>0.74</v>
+        <v>0.7383</v>
       </c>
       <c r="M6" s="1"/>
     </row>
@@ -419,34 +416,34 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0.7717</v>
+        <v>0.8104</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.76</v>
+        <v>0.7701</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>0.735</v>
+        <v>0.814</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0.7767</v>
+        <v>0.7755</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>0.7817</v>
+        <v>0.8055</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0.7133</v>
+        <v>0.8173</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>0.7383</v>
+        <v>0.7562</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0.76</v>
+        <v>0.7384</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>0.7883</v>
+        <v>0.7647</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.7783</v>
+        <v>0.7307</v>
       </c>
       <c r="M7" s="1"/>
     </row>
@@ -458,34 +455,34 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0.765</v>
+        <v>0.7913</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.7513</v>
+        <v>0.7475</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.7463</v>
+        <v>0.7575</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.775</v>
+        <v>0.7863</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.7675</v>
+        <v>0.7875</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0.7888</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>0.7863</v>
+        <v>0.7513</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>0.7688</v>
+        <v>0.77</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0.7663</v>
+        <v>0.7775</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.7775</v>
+        <v>0.7713</v>
       </c>
       <c r="M8" s="1"/>
     </row>
@@ -494,34 +491,34 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0.7662</v>
+        <v>0.7795</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0.7812</v>
+        <v>0.7835</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>0.725</v>
+        <v>0.7926</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>0.735</v>
+        <v>0.7717</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.7787</v>
+        <v>0.7755</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>0.7675</v>
+        <v>0.8032</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>0.7787</v>
+        <v>0.7798</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>0.765</v>
+        <v>0.8051</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>0.7725</v>
+        <v>0.7604</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.7662</v>
+        <v>0.7568</v>
       </c>
       <c r="M9" s="1"/>
     </row>
@@ -533,34 +530,34 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0.746</v>
+        <v>0.742</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.776</v>
+        <v>0.743</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0.765</v>
+        <v>0.789</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>0.764</v>
+        <v>0.769</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0.766</v>
+        <v>0.782</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0.768</v>
+        <v>0.758</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>0.786</v>
+        <v>0.782</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>0.775</v>
+        <v>0.793</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>0.752</v>
+        <v>0.772</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0.748</v>
+        <v>0.78</v>
       </c>
       <c r="M10" s="1"/>
     </row>
@@ -569,34 +566,34 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.776</v>
+        <v>0.7523</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.779</v>
+        <v>0.7682</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>0.785</v>
+        <v>0.7732</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0.773</v>
+        <v>0.793</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.773</v>
+        <v>0.7813</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>761</v>
+        <v>0.7474</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>0.79</v>
+        <v>0.757</v>
       </c>
       <c r="J11" s="1" t="n">
         <v>0.769</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>0.764</v>
+        <v>0.7806</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.775</v>
+        <v>0.7671</v>
       </c>
       <c r="M11" s="1"/>
     </row>
@@ -619,13 +616,10 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10:L11"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -679,34 +673,34 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>0.58</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>1</v>
+        <v>0.465</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>1</v>
+        <v>0.505</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>1</v>
+        <v>0.445</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>1</v>
+        <v>0.505</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>1</v>
+        <v>0.465</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>1</v>
+        <v>0.575</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>1</v>
+        <v>0.455</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="M2" s="1"/>
     </row>
@@ -715,34 +709,34 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1</v>
+        <v>0.515</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>1</v>
+        <v>0.55</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>1</v>
+        <v>0.475</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>1</v>
+        <v>0.53</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>1</v>
+        <v>0.455</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>1</v>
+        <v>0.545</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>1</v>
+        <v>0.47</v>
       </c>
       <c r="M3" s="1"/>
     </row>
@@ -754,34 +748,34 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1</v>
+        <v>0.5075</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>1</v>
+        <v>0.4825</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1</v>
+        <v>0.4825</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>0.475</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>1</v>
+        <v>0.4925</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>1</v>
+        <v>0.5175</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>1</v>
+        <v>0.485</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>1</v>
+        <v>0.475</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="M4" s="1"/>
     </row>
@@ -790,34 +784,34 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>1</v>
+        <v>0.4475</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>1</v>
+        <v>0.515</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>1</v>
+        <v>0.475</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>0.46</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>1</v>
+        <v>0.49</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>1</v>
+        <v>0.4925</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>1</v>
+        <v>0.485</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>1</v>
+        <v>0.4825</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>1</v>
+        <v>0.5175</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>1</v>
+        <v>0.4925</v>
       </c>
       <c r="M5" s="1"/>
     </row>
@@ -829,34 +823,34 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>0.4783</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>1</v>
+        <v>0.505</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>1</v>
+        <v>0.497</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>1</v>
+        <v>0.5017</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>1</v>
+        <v>0.515</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>1</v>
+        <v>0.515</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>1</v>
+        <v>0.475</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>1</v>
+        <v>0.505</v>
       </c>
       <c r="M6" s="1"/>
     </row>
@@ -865,34 +859,34 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>1</v>
+        <v>0.4817</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>1</v>
+        <v>0.5233</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>1</v>
+        <v>0.5033</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>1</v>
+        <v>0.515</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>1</v>
+        <v>0.497</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>1</v>
+        <v>0.4783</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>1</v>
+        <v>0.5217</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>1</v>
+        <v>0.4983</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>1</v>
+        <v>0.4917</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>1</v>
+        <v>0.5017</v>
       </c>
       <c r="M7" s="1"/>
     </row>
@@ -904,34 +898,34 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1</v>
+        <v>0.5313</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1</v>
+        <v>0.4775</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>1</v>
+        <v>0.5125</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>0.5038</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>1</v>
+        <v>0.5413</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>1</v>
+        <v>0.5163</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>1</v>
+        <v>0.4863</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>1</v>
+        <v>0.5263</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>1</v>
+        <v>0.5113</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>1</v>
+        <v>0.505</v>
       </c>
       <c r="M8" s="1"/>
     </row>
@@ -940,34 +934,34 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1</v>
+        <v>0.5088</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>1</v>
+        <v>0.4787</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>1</v>
+        <v>0.5038</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>1</v>
+        <v>0.4825</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>1</v>
+        <v>0.5125</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>1</v>
+        <v>0.4787</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>1</v>
+        <v>0.4837</v>
       </c>
       <c r="M9" s="1"/>
     </row>
@@ -979,34 +973,34 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>1</v>
+        <v>0.519</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>1</v>
+        <v>0.502</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>1</v>
+        <v>0.498</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
+        <v>0.481</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>1</v>
+        <v>0.473</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>1</v>
+        <v>0.483</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>1</v>
+        <v>0.47</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>1</v>
+        <v>0.506</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>1</v>
+        <v>0.524</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>1</v>
+        <v>0.497</v>
       </c>
       <c r="M10" s="1"/>
     </row>
@@ -1015,34 +1009,34 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1</v>
+        <v>0.488</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1</v>
+        <v>0.499</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>1</v>
+        <v>0.484</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>1</v>
+        <v>0.533</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>1</v>
+        <v>0.506</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>1</v>
+        <v>0.501</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>1</v>
+        <v>0.513</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>1</v>
+        <v>0.495</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>1</v>
+        <v>0.52</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>1</v>
+        <v>0.496</v>
       </c>
       <c r="M11" s="1"/>
     </row>

</xml_diff>